<commit_message>
added placement_analysis data for my colleges
</commit_message>
<xml_diff>
--- a/Files/college_info/all_colleges/OUCE/OUCE_placements.xlsx
+++ b/Files/college_info/all_colleges/OUCE/OUCE_placements.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad Arshad Ali\Dropbox\Programming\KMIT\Projects\group\python project on dataset (1st year 2nd sem)\files\OCUE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad Arshad Ali\Dropbox\Programming\KMIT\Projects\group\python project on dataset (1st year 2nd sem)\files\all_colleges\OUCE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E889B6EE-4B1E-4124-80AC-B7A5C623F7D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9680225-F806-443C-8311-C59CF980123B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -656,7 +656,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -767,7 +767,7 @@
     </row>
     <row r="8" spans="1:4" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>14</v>
@@ -781,7 +781,7 @@
     </row>
     <row r="9" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>9</v>
@@ -795,7 +795,7 @@
     </row>
     <row r="10" spans="1:4" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>11</v>
@@ -809,7 +809,7 @@
     </row>
     <row r="11" spans="1:4" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>15</v>
@@ -823,7 +823,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>5</v>
@@ -837,7 +837,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>3</v>
@@ -851,7 +851,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>8</v>
@@ -865,7 +865,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>12</v>
@@ -879,7 +879,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>13</v>
@@ -893,7 +893,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>16</v>
@@ -907,7 +907,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>17</v>
@@ -921,7 +921,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>2</v>
@@ -935,7 +935,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>4</v>
@@ -948,8 +948,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A24">
-    <sortCondition ref="A1:A24"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A23">
+    <sortCondition ref="A1:A23"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>